<commit_message>
edits to eml for edi
</commit_message>
<xml_diff>
--- a/4.project.113/Metadata.xlsx
+++ b/4.project.113/Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/palomacartwright/Documents/EDI/felmer-phd-data/4.project.113/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2BC7B2-FDC0-4749-A528-CAEF3392CD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4753EDE9-C4EF-C343-9C97-4EEA70A192D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-640" yWindow="-23500" windowWidth="32420" windowHeight="20020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27840" windowHeight="17500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -481,7 +481,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3502" uniqueCount="1584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3503" uniqueCount="1585">
   <si>
     <t>csv_E</t>
   </si>
@@ -5233,6 +5233,9 @@
   </si>
   <si>
     <t>Algae A (percent cover)</t>
+  </si>
+  <si>
+    <t>urlpath</t>
   </si>
 </sst>
 </file>
@@ -5797,7 +5800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
@@ -13866,10 +13869,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -13883,7 +13886,7 @@
     <col min="7" max="7" width="49.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>820</v>
       </c>
@@ -13905,8 +13908,11 @@
       <c r="G1" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>113</v>
       </c>
@@ -13929,7 +13935,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>113</v>
       </c>
@@ -13952,7 +13958,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>113</v>
       </c>
@@ -13975,7 +13981,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>113</v>
       </c>
@@ -13998,7 +14004,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="16">
+    <row r="6" spans="1:8" s="1" customFormat="1" ht="16">
       <c r="A6" s="1">
         <v>113</v>
       </c>
@@ -14021,7 +14027,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>113</v>
       </c>
@@ -14044,7 +14050,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>113</v>
       </c>
@@ -14067,7 +14073,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>113</v>
       </c>
@@ -14090,7 +14096,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>113</v>
       </c>
@@ -14151,8 +14157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K276"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F187" sqref="F187"/>
     </sheetView>
   </sheetViews>
@@ -19673,7 +19679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>

</xml_diff>